<commit_message>
Updated the order of the supplemental tables to reflect the order they are in in the manuscript.
</commit_message>
<xml_diff>
--- a/products/TIR_manuscript/Supplemental_Tables/Supplemental_Table_8.xlsx
+++ b/products/TIR_manuscript/Supplemental_Tables/Supplemental_Table_8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work_Files\GCMP_TIR\immunity_microbiome\Supplemental_Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC87D4A-0691-4782-A1C4-DD10FD1EC69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279132DF-2739-493D-9E6A-E0283044B50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3828" yWindow="2604" windowWidth="17280" windowHeight="8964" xr2:uid="{1D9A66A8-7322-49B3-B858-11998F327895}"/>
+    <workbookView xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8964" xr2:uid="{1D9A66A8-7322-49B3-B858-11998F327895}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S8A" sheetId="1" r:id="rId1"/>
@@ -23,20 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="32">
   <si>
     <t>Immune_Trait</t>
   </si>
@@ -53,13 +45,19 @@
     <t>ln_asvs</t>
   </si>
   <si>
+    <t>TIR_total_unique</t>
+  </si>
+  <si>
     <t>gini_index</t>
   </si>
   <si>
-    <t>IL1R</t>
-  </si>
-  <si>
-    <t>TLR</t>
+    <t>TIR_total</t>
+  </si>
+  <si>
+    <t>LRR_total</t>
+  </si>
+  <si>
+    <t>LRR_total_unique</t>
   </si>
   <si>
     <t>ln_asvs_mucus</t>
@@ -80,6 +78,12 @@
     <t>gini_index_tissue</t>
   </si>
   <si>
+    <t>IG_total</t>
+  </si>
+  <si>
+    <t>IG_total_unique</t>
+  </si>
+  <si>
     <t>PIC_Model</t>
   </si>
   <si>
@@ -101,28 +105,25 @@
     <t>lm(y_trait_positive ~ x_trait_positive -1)</t>
   </si>
   <si>
-    <t>Table S8A: Phylogenetic comparison of IL-1R and TLR gene family copies vs Alpha Diversity in all compartments</t>
-  </si>
-  <si>
-    <t>Phylogenetic independent contranst results for IL-1R and TLR gene families for ln ASVs and Gini Index in all compartments combined for the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by immune trait (eg IL-1R or TLR).</t>
-  </si>
-  <si>
-    <t>Table S8B: Phylogenetic comparison of IL-1R and TLR gene family copies vs. Alpha Diversity in the mucus compartment</t>
-  </si>
-  <si>
-    <t>Phylogenetic independent contranst results for IL-1R and TLR gene families for ln ASVs and Gini Index the mucus compartment combined for the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by immune trait (eg IL-1R or TLR).</t>
-  </si>
-  <si>
-    <t>Table S8C: Phylogenetic comparison of IL-1R and TLR gene family copies vs. Alpha Diversity in the tissue compartment</t>
-  </si>
-  <si>
-    <t>Phylogenetic independent contranst results for IL-1R and TLR gene families for ln ASVs and Gini Index the tissue compartment combined for the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by immune trait (eg IL-1R or TLR).</t>
-  </si>
-  <si>
-    <t>Table S8D: Phylogenetic comparison of IL-1R and TLR gene family copies vs Alpha Diversity in the skeleton compartment</t>
-  </si>
-  <si>
-    <t>Phylogenetic independent contranst results for IL-1R and TLR gene families for ln ASVs and Gini Index the skeleton compartment combined for the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by immune trait (eg IL-1R or TLR).</t>
+    <t>Phylogenetic independent contranst results for TIR, LRR, and Ig domains for ln ASVs and Gini Index in the mucus compartment in the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by domain analyzed (eg TIR total or TIR total unique).</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for TIR, LRR, and Ig domains for ln ASVs and Gini Index in all compartments combined in the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by domain analyzed (eg TIR total or TIR total unique).</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for TIR, LRR, and Ig domains for ln ASVs and Gini Index in the skeletal compartment in the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by domain analyzed (eg TIR total or TIR total unique).</t>
+  </si>
+  <si>
+    <t>Table S8A: Phylogenetic comparison of TIR, LRR, and Ig domains vs Alpha Diversity in all compartments for all and unique isoforms</t>
+  </si>
+  <si>
+    <t>Table S8B: Phylogenic comarison of TIR, LRR, and Ig domains vs. Alpha Diversity in the mucus compatment for all and unique isoforms</t>
+  </si>
+  <si>
+    <t>Table S8C: Phylogenetic comparison of TIR, LRR, and Ig domains vs. Alpha Diversity in the tissue compartment for all and unique isoforms</t>
+  </si>
+  <si>
+    <t>Table S8D: Phylogenetic comparison of TIR, LRR, and Ig domains vs. Alpha Diversity in the skeleton compartment for all and unique isoforms</t>
   </si>
 </sst>
 </file>
@@ -207,8 +208,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,28 +525,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F45E0DC-CD8B-4D76-B79F-EC971B0A48B7}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="13.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -557,9 +558,9 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -585,22 +586,22 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -608,7 +609,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3">
         <v>183</v>
@@ -617,30 +618,30 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4">
-        <v>5.1400000000000003E-5</v>
+        <v>24</v>
+      </c>
+      <c r="F4" s="3">
+        <v>6.4588704999999996E-2</v>
       </c>
       <c r="G4" s="3">
-        <v>0.85173555300000003</v>
+        <v>0.32991621799999998</v>
       </c>
       <c r="H4" s="3">
-        <v>1.64E-3</v>
+        <v>1</v>
       </c>
       <c r="I4" s="3">
-        <v>1.5399999999999999E-3</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="J4" s="3">
-        <v>5.4799999999999998E-4</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="C5" s="3">
         <v>183</v>
@@ -649,27 +650,27 @@
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4">
-        <v>2.3E-5</v>
+        <v>24</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9.5520780000000003E-3</v>
       </c>
       <c r="G5" s="3">
-        <v>0.87562726000000002</v>
+        <v>0.54427109200000001</v>
       </c>
       <c r="H5" s="3">
-        <v>7.1299999999999998E-4</v>
+        <v>0.29611441799999999</v>
       </c>
       <c r="I5" s="3">
-        <v>6.8999999999999997E-4</v>
+        <v>0.219697794</v>
       </c>
       <c r="J5" s="3">
-        <v>3.5649999999999999E-4</v>
+        <v>3.2901602000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
@@ -681,27 +682,27 @@
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3">
-        <v>1.1916299999999999E-3</v>
+        <v>8.2790450000000005E-3</v>
       </c>
       <c r="G6" s="3">
-        <v>0.70665031300000003</v>
+        <v>0.55764336800000003</v>
       </c>
       <c r="H6" s="3">
-        <v>3.8100000000000002E-2</v>
+        <v>0.25665039499999998</v>
       </c>
       <c r="I6" s="3">
-        <v>3.3399999999999999E-2</v>
+        <v>0.19869708</v>
       </c>
       <c r="J6" s="3">
-        <v>7.6299999999999996E-3</v>
+        <v>3.2081299000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
@@ -713,22 +714,342 @@
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3">
-        <v>1.80478E-4</v>
+        <v>2.1276403999999999E-2</v>
       </c>
       <c r="G7" s="3">
-        <v>0.80494611199999999</v>
+        <v>0.462630035</v>
       </c>
       <c r="H7" s="3">
-        <v>5.5948179999999997E-3</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="I7" s="3">
-        <v>5.0533840000000002E-3</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="J7" s="3">
-        <v>1.3987050000000001E-3</v>
+        <v>8.5099999999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>183</v>
+      </c>
+      <c r="D8" s="3">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.504291398</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5.1007941000000001E-2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>183</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.25533713000000002</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.140879695</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.37692624000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>183</v>
+      </c>
+      <c r="D10" s="3">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.72117421199999998</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1.4846666999999999E-2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.79844287800000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <v>183</v>
+      </c>
+      <c r="D11" s="3">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.87110785800000001</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3.0869909999999999E-3</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>183</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.504291398</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5.1007941000000001E-2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3">
+        <v>183</v>
+      </c>
+      <c r="D13" s="3">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.25533713000000002</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.140879695</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.37692624000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3">
+        <v>183</v>
+      </c>
+      <c r="D14" s="3">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.28127911900000002</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.127377352</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3">
+        <v>183</v>
+      </c>
+      <c r="D15" s="3">
+        <v>11</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3">
+        <v>9.721581E-2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.27569654500000002</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.188355632</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3">
+        <v>183</v>
+      </c>
+      <c r="D16" s="3">
+        <v>11</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.64374768500000001</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2.4802698000000001E-2</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3">
+        <v>183</v>
+      </c>
+      <c r="D17" s="3">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="G17" s="3">
+        <v>6.7649099999999998E-4</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.939492349</v>
       </c>
     </row>
   </sheetData>
@@ -742,52 +1063,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6B1665-DC4B-4E92-B286-BE4598BBAC53}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.44140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="12.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -803,45 +1123,45 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="D4" s="3">
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3">
-        <v>0.10860603000000001</v>
+        <v>0.79575285200000001</v>
       </c>
       <c r="G4" s="3">
-        <v>0.260593874</v>
+        <v>7.8379060000000004E-3</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
@@ -850,62 +1170,62 @@
         <v>0.97799999999999998</v>
       </c>
       <c r="J4" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.92900000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3">
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3">
-        <v>3.2290447999999999E-2</v>
+        <v>0.109152324</v>
       </c>
       <c r="G5" s="3">
-        <v>0.41541878100000001</v>
+        <v>0.25990627999999999</v>
       </c>
       <c r="H5" s="3">
         <v>1</v>
       </c>
       <c r="I5" s="3">
-        <v>0.64580895999999999</v>
+        <v>0.939492349</v>
       </c>
       <c r="J5" s="3">
-        <v>8.3416990999999996E-2</v>
+        <v>0.199042473</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" s="3">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3">
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3">
-        <v>0.35081044900000002</v>
+        <v>0.108598746</v>
       </c>
       <c r="G6" s="3">
-        <v>9.7140392000000006E-2</v>
+        <v>0.260603064</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -914,39 +1234,231 @@
         <v>0.97799999999999998</v>
       </c>
       <c r="J6" s="3">
-        <v>0.624</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>61</v>
+      </c>
+      <c r="D7" s="3">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.14278596199999999</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.222698122</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.24590915699999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3">
-        <v>183</v>
-      </c>
-      <c r="D7" s="3">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="3">
-        <v>2.5839909000000001E-2</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.44104193400000002</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.80103717900000004</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.56094891300000005</v>
-      </c>
-      <c r="J7" s="3">
-        <v>7.5278859000000004E-2</v>
+      <c r="C8" s="3">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.6760105000000001E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.48817787600000001</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.436</v>
+      </c>
+      <c r="J8" s="3">
+        <v>7.6600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.292627101</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.121894114</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.41233818799999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>61</v>
+      </c>
+      <c r="D10" s="3">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.233424146</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.15348113299999999</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3">
+        <v>7.1606011999999997E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.31648348500000001</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.158556169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3">
+        <v>61</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4.0810580000000003E-3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.61869589800000002</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2.18E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3">
+        <v>61</v>
+      </c>
+      <c r="D13" s="3">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.45314740599999997</v>
+      </c>
+      <c r="G13" s="3">
+        <v>6.3937659999999993E-2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.61076389499999995</v>
       </c>
     </row>
   </sheetData>
@@ -960,28 +1472,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6510655-78C3-47CB-9604-B91752936AA0}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -993,19 +1505,19 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+    <row r="2" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1021,45 +1533,45 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="D4" s="3">
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3">
-        <v>0.20216985500000001</v>
+        <v>0.65073908899999999</v>
       </c>
       <c r="G4" s="3">
-        <v>0.173754413</v>
+        <v>2.3782548000000001E-2</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
@@ -1068,30 +1580,30 @@
         <v>0.97799999999999998</v>
       </c>
       <c r="J4" s="3">
-        <v>0.498</v>
+        <v>0.92900000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="D5" s="3">
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3">
-        <v>0.67760886200000003</v>
+        <v>0.64209839800000001</v>
       </c>
       <c r="G5" s="3">
-        <v>2.0091504E-2</v>
+        <v>2.5047033E-2</v>
       </c>
       <c r="H5" s="3">
         <v>1</v>
@@ -1105,25 +1617,25 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="D6" s="3">
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3">
-        <v>0.35023510699999999</v>
+        <v>0.97056416499999998</v>
       </c>
       <c r="G6" s="3">
-        <v>9.7360884999999994E-2</v>
+        <v>1.59908E-4</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -1132,39 +1644,231 @@
         <v>0.97799999999999998</v>
       </c>
       <c r="J6" s="3">
-        <v>0.624</v>
+        <v>0.97799999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="D7" s="3">
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3">
-        <v>0.917102525</v>
+        <v>2.6711853000000001E-2</v>
       </c>
       <c r="G7" s="3">
-        <v>1.2715300000000001E-3</v>
+        <v>0.43728468100000001</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
+        <v>0.82806744300000001</v>
       </c>
       <c r="I7" s="3">
-        <v>0.939492349</v>
+        <v>0.56094891300000005</v>
       </c>
       <c r="J7" s="3">
-        <v>0.939492349</v>
+        <v>7.5278859000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>62</v>
+      </c>
+      <c r="D8" s="3">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.82016300600000003</v>
+      </c>
+      <c r="G8" s="3">
+        <v>6.0511749999999998E-3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <v>62</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.0780059999999999E-3</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.66959555900000001</v>
+      </c>
+      <c r="H9" s="3">
+        <v>6.4418186000000002E-2</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5.6106162000000001E-2</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.123423E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>62</v>
+      </c>
+      <c r="D10" s="3">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.84836540500000002</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4.2844099999999998E-3</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <v>62</v>
+      </c>
+      <c r="D11" s="3">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3">
+        <v>4.7647965E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.36848916100000001</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.90531133500000005</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.11362207000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3">
+        <v>62</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.688031689</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.8755217000000001E-2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3">
+        <v>62</v>
+      </c>
+      <c r="D13" s="3">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2.174367E-3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.66638740500000004</v>
+      </c>
+      <c r="H13" s="3">
+        <v>6.7405377000000002E-2</v>
+      </c>
+      <c r="I13" s="3">
+        <v>5.6533541999999999E-2</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.123423E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1178,28 +1882,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80615E1-7162-4E4A-9B78-187BC642500B}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="13.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1211,19 +1915,19 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+    <row r="2" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1239,150 +1943,342 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
-        <v>183</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3">
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4">
-        <v>6.3900000000000004E-7</v>
+        <v>24</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2.5224600000000002E-4</v>
       </c>
       <c r="G4" s="3">
-        <v>0.94354677300000001</v>
+        <v>0.79022158799999997</v>
       </c>
       <c r="H4" s="3">
-        <v>2.05E-5</v>
+        <v>8.0700000000000008E-3</v>
       </c>
       <c r="I4" s="3">
-        <v>2.05E-5</v>
+        <v>7.3200000000000001E-3</v>
       </c>
       <c r="J4" s="3">
-        <v>2.05E-5</v>
+        <v>2.0200000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>183</v>
+        <v>63</v>
       </c>
       <c r="D5" s="3">
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.1199999999999999E-5</v>
+        <v>24</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4.884668E-3</v>
       </c>
       <c r="G5" s="3">
-        <v>0.89393824600000005</v>
+        <v>0.60396066599999998</v>
       </c>
       <c r="H5" s="3">
-        <v>3.4719999999999998E-4</v>
+        <v>0.15142470799999999</v>
       </c>
       <c r="I5" s="3">
-        <v>3.4719999999999998E-4</v>
+        <v>0.12211669999999999</v>
       </c>
       <c r="J5" s="3">
-        <v>3.4719999999999998E-4</v>
+        <v>2.1632101000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>183</v>
+        <v>63</v>
       </c>
       <c r="D6" s="3">
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="4">
-        <v>5.8499999999999999E-6</v>
+        <v>24</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.233521642</v>
       </c>
       <c r="G6" s="3">
-        <v>0.90798204199999999</v>
+        <v>0.15342235800000001</v>
       </c>
       <c r="H6" s="3">
-        <v>1.8699999999999999E-4</v>
+        <v>1</v>
       </c>
       <c r="I6" s="3">
-        <v>1.8100000000000001E-4</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="J6" s="3">
-        <v>9.3599999999999998E-5</v>
+        <v>0.498</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>183</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3">
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="4">
-        <v>8.8599999999999999E-5</v>
+        <v>24</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.228917697</v>
       </c>
       <c r="G7" s="3">
-        <v>0.832967597</v>
+        <v>0.156226066</v>
       </c>
       <c r="H7" s="3">
-        <v>2.7466000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="I7" s="3">
-        <v>2.5693999999999999E-3</v>
+        <v>0.939492349</v>
       </c>
       <c r="J7" s="3">
-        <v>9.1553299999999995E-4</v>
+        <v>0.37349729500000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>63</v>
+      </c>
+      <c r="D8" s="3">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.83933318599999995</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4.8159789999999997E-3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <v>63</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.69034878399999999</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1.8465229999999999E-2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.79844287800000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>63</v>
+      </c>
+      <c r="D10" s="3">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.10186967199999999</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.26934159800000002</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <v>63</v>
+      </c>
+      <c r="D11" s="3">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3">
+        <v>8.2082454999999999E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.298440288</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.169637074</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3">
+        <v>63</v>
+      </c>
+      <c r="D12" s="3">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.97842166399999997</v>
+      </c>
+      <c r="G12" s="4">
+        <v>8.5900000000000001E-5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.89654858400000004</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1.9835270000000001E-3</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.939492349</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.939492349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>